<commit_message>
Traitement de la data reçue par le fichier Excel
</commit_message>
<xml_diff>
--- a/public/documents/StudentRegister.xlsx
+++ b/public/documents/StudentRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\laravel_learning\20190226_TDN_Laravel\tdn_laravel_2020\public\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD712DB-9599-438D-9354-C2743BE4437E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05FB771-8159-4C8A-9EA6-CB4B9D5B20AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Ingesup Ynov</t>
+  </si>
+  <si>
+    <t>Marcus Thomas</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Paris HEC</t>
   </si>
 </sst>
 </file>
@@ -385,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,6 +442,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>